<commit_message>
Updated Export Prototype (Screenings-Client list)
</commit_message>
<xml_diff>
--- a/Documentation/Export Prototype/Screenings/ExportScreeningClientList.xlsx
+++ b/Documentation/Export Prototype/Screenings/ExportScreeningClientList.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="16925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17329"/>
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Teh Kaixin\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Teh Kaixin\Desktop\FYP GIT\Ulink\Documentation\Export Prototype\Screenings\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="13">
   <si>
     <t>Name</t>
   </si>
@@ -60,6 +60,9 @@
   </si>
   <si>
     <t>charles@yahoo.com</t>
+  </si>
+  <si>
+    <t>S/N</t>
   </si>
 </sst>
 </file>
@@ -436,74 +439,86 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.85546875" customWidth="1"/>
-    <col min="2" max="2" width="11.85546875" customWidth="1"/>
-    <col min="3" max="3" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.85546875" customWidth="1"/>
+    <col min="3" max="3" width="11.85546875" customWidth="1"/>
+    <col min="4" max="4" width="19.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>6</v>
       </c>
       <c r="B1" s="2"/>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="C3" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="D3" s="3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>1</v>
+      </c>
+      <c r="B4" t="s">
         <v>3</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C4" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="D4" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>2</v>
+      </c>
+      <c r="B5" t="s">
         <v>7</v>
       </c>
-      <c r="B5" t="s">
+      <c r="C5" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="D5" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>3</v>
+      </c>
+      <c r="B6" t="s">
         <v>10</v>
       </c>
-      <c r="B6" t="s">
+      <c r="C6" t="s">
         <v>4</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="D6" s="1" t="s">
         <v>11</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C4" r:id="rId1"/>
-    <hyperlink ref="C5" r:id="rId2"/>
-    <hyperlink ref="C6" r:id="rId3"/>
+    <hyperlink ref="D4" r:id="rId1"/>
+    <hyperlink ref="D5" r:id="rId2"/>
+    <hyperlink ref="D6" r:id="rId3"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>